<commit_message>
Se actualiza la evaluacion de herramientas
</commit_message>
<xml_diff>
--- a/Informes/Requerimientos.xlsx
+++ b/Informes/Requerimientos.xlsx
@@ -4,13 +4,15 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20640" windowHeight="11760" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20640" windowHeight="11760" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Req. F" sheetId="2" r:id="rId1"/>
     <sheet name="Req. NF" sheetId="4" r:id="rId2"/>
-    <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
-    <sheet name="Hoja1" sheetId="1" r:id="rId4"/>
+    <sheet name="Glosario" sheetId="3" r:id="rId3"/>
+    <sheet name="Herramientas" sheetId="1" r:id="rId4"/>
+    <sheet name="Evaluacion Herramientas" sheetId="5" r:id="rId5"/>
+    <sheet name="Hoja2" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="140000" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="119">
   <si>
     <t>Herramientas para la Asignación de Tareas</t>
   </si>
@@ -331,12 +333,165 @@
   <si>
     <t>Los desarrolladores podran ingresar las tareas diarias que han realizado relacionadas a sus proyectos.</t>
   </si>
+  <si>
+    <t>Nombre Herramienta</t>
+  </si>
+  <si>
+    <t>Referencia</t>
+  </si>
+  <si>
+    <t>Codigo Libre</t>
+  </si>
+  <si>
+    <t>http://www.hesk.com/</t>
+  </si>
+  <si>
+    <t>Hesk</t>
+  </si>
+  <si>
+    <t>Herramientas</t>
+  </si>
+  <si>
+    <t>osticket</t>
+  </si>
+  <si>
+    <t>Help Desk</t>
+  </si>
+  <si>
+    <t>Escrito en Java</t>
+  </si>
+  <si>
+    <t>Puede ser desplegado en Glassfish 3.1.1</t>
+  </si>
+  <si>
+    <t>Puede utilizar SQL Server</t>
+  </si>
+  <si>
+    <t>Permite generación de solicitudes</t>
+  </si>
+  <si>
+    <t>Genera numero de consulta para el seguimiento de la solicitud</t>
+  </si>
+  <si>
+    <t>Permite la subdivision por areas</t>
+  </si>
+  <si>
+    <t>Es posible integrarlo con el sistema de autenticacion SSO de la universidad.</t>
+  </si>
+  <si>
+    <t>El solicitante puede ver un historial de sus solicitudes</t>
+  </si>
+  <si>
+    <t>Permite la reasignación de tareas a otras areas.</t>
+  </si>
+  <si>
+    <t>Soporta el manejo de roles</t>
+  </si>
+  <si>
+    <t>Existe la posibilidade de priorisar tareas</t>
+  </si>
+  <si>
+    <t>Existe la posibilidad de establecer fecha de termino de las tareas.</t>
+  </si>
+  <si>
+    <t>Se generan alarmas para las tareas atrasadas.</t>
+  </si>
+  <si>
+    <t>Se puede modificar el estado de las solicitudes, entre Asignada, Pendiente, En ejecucion o Finalizada (o equivalentes)</t>
+  </si>
+  <si>
+    <t>Se puede enviar notificacion por correo electronico de la finalizacion de una tarea.</t>
+  </si>
+  <si>
+    <t>Version Gratuita</t>
+  </si>
+  <si>
+    <t>Version de Pago</t>
+  </si>
+  <si>
+    <t>SI</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>NO (PHP)</t>
+  </si>
+  <si>
+    <t>NO (MySQL)</t>
+  </si>
+  <si>
+    <r>
+      <t>Username: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF4A5571"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>Administrator</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Password: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF4A5571"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>admin</t>
+    </r>
+  </si>
+  <si>
+    <t>Envia numero de solicitud de consulta por email</t>
+  </si>
+  <si>
+    <t>Automaticamente NO, debe pedirse el envio indicando que ha olvidado el numero</t>
+  </si>
+  <si>
+    <t>Lo mas similar es dividir en categorias</t>
+  </si>
+  <si>
+    <t>Permite mover tareas a otra categoria</t>
+  </si>
+  <si>
+    <t>Soporta manejo de permisos</t>
+  </si>
+  <si>
+    <t>Se puede asignar responsables a las tareas</t>
+  </si>
+  <si>
+    <t>Se pueden ver estadisticas de las actividades que se encuentra realizando cada persona.</t>
+  </si>
+  <si>
+    <t>Solo administrador y solo ve asignadas y respondidas (no de en ejecucion ni pendientes, ni el detalle de cuales son</t>
+  </si>
+  <si>
+    <t>Lenguaje español</t>
+  </si>
+  <si>
+    <t>Ingles por defecto (Español es necesario descargarlo aparte y solo esta disponible asta la version 2.1)</t>
+  </si>
+  <si>
+    <t>SI (complicado)</t>
+  </si>
+  <si>
+    <t>Existe un perfil encargado de recibir las tareas del area y asignarles responsables</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -392,8 +547,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF4A5571"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF4A5571"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -406,8 +580,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -498,8 +678,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -509,8 +702,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -555,23 +749,29 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -581,9 +781,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -593,15 +790,43 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="9"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="10">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="9" builtinId="8"/>
     <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="6" builtinId="9" hidden="1"/>
@@ -942,8 +1167,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B41" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="F46" sqref="F46"/>
+    <sheetView topLeftCell="B19" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -967,7 +1192,7 @@
       <c r="C4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="26" t="s">
+      <c r="D4" s="20" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1203,54 +1428,54 @@
       </c>
     </row>
     <row r="26" spans="2:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="17">
+      <c r="B26" s="22">
         <v>22</v>
       </c>
-      <c r="C26" s="18" t="s">
+      <c r="C26" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="D26" s="27" t="s">
+      <c r="D26" s="28" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="27" spans="2:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="19"/>
-      <c r="C27" s="20" t="s">
+      <c r="B27" s="23"/>
+      <c r="C27" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="D27" s="28"/>
+      <c r="D27" s="29"/>
     </row>
     <row r="28" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="21"/>
-      <c r="C28" s="22" t="s">
+      <c r="B28" s="24"/>
+      <c r="C28" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="D28" s="29"/>
+      <c r="D28" s="30"/>
     </row>
     <row r="29" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="23">
+      <c r="B29" s="25">
         <v>23</v>
       </c>
-      <c r="C29" s="18" t="s">
+      <c r="C29" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="D29" s="27" t="s">
+      <c r="D29" s="28" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="30" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="24"/>
-      <c r="C30" s="20" t="s">
+      <c r="B30" s="26"/>
+      <c r="C30" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="D30" s="28"/>
+      <c r="D30" s="29"/>
     </row>
     <row r="31" spans="2:4" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="25"/>
-      <c r="C31" s="22" t="s">
+      <c r="B31" s="27"/>
+      <c r="C31" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="D31" s="29"/>
+      <c r="D31" s="30"/>
     </row>
     <row r="32" spans="2:4" ht="42.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="15">
@@ -1460,8 +1685,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D20"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11:D16"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1611,10 +1836,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C11"/>
+  <dimension ref="B2:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1675,7 +1900,7 @@
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B10" s="30" t="s">
+      <c r="B10" s="21" t="s">
         <v>69</v>
       </c>
       <c r="C10" s="16" t="s">
@@ -1683,11 +1908,16 @@
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B11" s="30" t="s">
+      <c r="B11" s="21" t="s">
         <v>70</v>
       </c>
       <c r="C11" s="16" t="s">
         <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B13" s="34" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -1702,25 +1932,407 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2"/>
+  <dimension ref="B2:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.125" customWidth="1"/>
+    <col min="2" max="2" width="14.875" customWidth="1"/>
+    <col min="3" max="3" width="28.5" customWidth="1"/>
+    <col min="4" max="4" width="31.625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
+    <row r="3" spans="2:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="2:4" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D5" s="31" t="s">
+        <v>79</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D5" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:F36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.25" customWidth="1"/>
+    <col min="2" max="2" width="32.625" customWidth="1"/>
+    <col min="3" max="3" width="32.75" style="32" customWidth="1"/>
+    <col min="4" max="4" width="11" style="32"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C3" s="33" t="s">
+        <v>81</v>
+      </c>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C4" s="42" t="s">
+        <v>80</v>
+      </c>
+      <c r="D4" s="42" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="39" t="s">
+        <v>99</v>
+      </c>
+      <c r="C5" s="36" t="s">
+        <v>101</v>
+      </c>
+      <c r="D5" s="36" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="39" t="s">
+        <v>100</v>
+      </c>
+      <c r="C6" s="36" t="s">
+        <v>101</v>
+      </c>
+      <c r="D6" s="36"/>
+    </row>
+    <row r="7" spans="2:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="39" t="s">
+        <v>78</v>
+      </c>
+      <c r="C7" s="36" t="s">
+        <v>101</v>
+      </c>
+      <c r="D7" s="36"/>
+    </row>
+    <row r="8" spans="2:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="C8" s="36" t="s">
+        <v>103</v>
+      </c>
+      <c r="D8" s="36" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" s="12" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B9" s="39" t="s">
+        <v>115</v>
+      </c>
+      <c r="C9" s="36" t="s">
+        <v>116</v>
+      </c>
+      <c r="D9" s="36" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="39"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="36"/>
+    </row>
+    <row r="11" spans="2:6" s="12" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B11" s="39" t="s">
+        <v>85</v>
+      </c>
+      <c r="C11" s="36" t="s">
+        <v>102</v>
+      </c>
+      <c r="D11" s="36" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="39" t="s">
+        <v>86</v>
+      </c>
+      <c r="C12" s="36" t="s">
+        <v>104</v>
+      </c>
+      <c r="D12" s="36" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="39" t="s">
+        <v>87</v>
+      </c>
+      <c r="C13" s="36" t="s">
+        <v>101</v>
+      </c>
+      <c r="D13" s="36" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" s="12" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B14" s="39" t="s">
+        <v>88</v>
+      </c>
+      <c r="C14" s="36" t="s">
+        <v>101</v>
+      </c>
+      <c r="D14" s="36" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" s="12" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B15" s="39" t="s">
+        <v>107</v>
+      </c>
+      <c r="C15" s="36" t="s">
+        <v>108</v>
+      </c>
+      <c r="D15" s="36" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="39" t="s">
+        <v>89</v>
+      </c>
+      <c r="C16" s="36" t="s">
+        <v>109</v>
+      </c>
+      <c r="D16" s="36" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" s="12" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="39" t="s">
+        <v>90</v>
+      </c>
+      <c r="C17" s="36" t="s">
+        <v>102</v>
+      </c>
+      <c r="D17" s="36" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" s="12" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B18" s="40" t="s">
+        <v>91</v>
+      </c>
+      <c r="C18" s="36" t="s">
+        <v>102</v>
+      </c>
+      <c r="D18" s="36" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" s="12" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B19" s="40" t="s">
+        <v>92</v>
+      </c>
+      <c r="C19" s="36" t="s">
+        <v>110</v>
+      </c>
+      <c r="D19" s="36" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="40" t="s">
+        <v>93</v>
+      </c>
+      <c r="C20" s="36" t="s">
+        <v>111</v>
+      </c>
+      <c r="D20" s="36" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" s="1" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+      <c r="B21" s="39" t="s">
+        <v>113</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" s="12" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B22" s="40" t="s">
+        <v>94</v>
+      </c>
+      <c r="C22" s="36" t="s">
+        <v>101</v>
+      </c>
+      <c r="D22" s="36" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" s="12" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B23" s="40" t="s">
+        <v>95</v>
+      </c>
+      <c r="C23" s="36" t="s">
+        <v>102</v>
+      </c>
+      <c r="D23" s="36"/>
+    </row>
+    <row r="24" spans="2:4" s="12" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B24" s="40" t="s">
+        <v>96</v>
+      </c>
+      <c r="C24" s="36" t="s">
+        <v>102</v>
+      </c>
+      <c r="D24" s="36"/>
+    </row>
+    <row r="25" spans="2:4" s="12" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+      <c r="B25" s="40" t="s">
+        <v>97</v>
+      </c>
+      <c r="C25" s="36" t="s">
+        <v>101</v>
+      </c>
+      <c r="D25" s="36" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" s="12" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B26" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="C26" s="36" t="s">
+        <v>102</v>
+      </c>
+      <c r="D26" s="36" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" s="12" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B27" s="41" t="s">
+        <v>112</v>
+      </c>
+      <c r="C27" s="36" t="s">
+        <v>102</v>
+      </c>
+      <c r="D27" s="36" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" s="12" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B28" s="35" t="s">
+        <v>118</v>
+      </c>
+      <c r="C28" s="36" t="s">
+        <v>102</v>
+      </c>
+      <c r="D28" s="36" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C29" s="37"/>
+      <c r="D29" s="37"/>
+    </row>
+    <row r="30" spans="2:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C30" s="37"/>
+      <c r="D30" s="37"/>
+    </row>
+    <row r="31" spans="2:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C31" s="37"/>
+      <c r="D31" s="37"/>
+    </row>
+    <row r="32" spans="2:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C32" s="37"/>
+      <c r="D32" s="37"/>
+    </row>
+    <row r="33" spans="3:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C33" s="37"/>
+      <c r="D33" s="37"/>
+    </row>
+    <row r="34" spans="3:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C34" s="37"/>
+      <c r="D34" s="37"/>
+    </row>
+    <row r="35" spans="3:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C35" s="37"/>
+      <c r="D35" s="37"/>
+    </row>
+    <row r="36" spans="3:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C36" s="37"/>
+      <c r="D36" s="37"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C3:F3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B4" s="38" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B5" s="38" t="s">
+        <v>106</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Se añaden algunos estándares
</commit_message>
<xml_diff>
--- a/Informes/Requerimientos.xlsx
+++ b/Informes/Requerimientos.xlsx
@@ -1,18 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20640" windowHeight="11760" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24600" windowHeight="14000" tabRatio="602" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Req. F" sheetId="2" r:id="rId1"/>
     <sheet name="Req. NF" sheetId="4" r:id="rId2"/>
     <sheet name="Glosario" sheetId="3" r:id="rId3"/>
     <sheet name="Herramientas" sheetId="1" r:id="rId4"/>
-    <sheet name="Evaluacion Herramientas" sheetId="5" r:id="rId5"/>
-    <sheet name="Hoja2" sheetId="6" r:id="rId6"/>
+    <sheet name="Evaluacion Herramienta HelpDesk" sheetId="6" r:id="rId5"/>
+    <sheet name="Evaluacion Herramienta SCM" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="140000" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="126">
   <si>
     <t>Herramientas para la Asignación de Tareas</t>
   </si>
@@ -340,18 +340,12 @@
     <t>Referencia</t>
   </si>
   <si>
-    <t>Codigo Libre</t>
-  </si>
-  <si>
     <t>http://www.hesk.com/</t>
   </si>
   <si>
     <t>Hesk</t>
   </si>
   <si>
-    <t>Herramientas</t>
-  </si>
-  <si>
     <t>osticket</t>
   </si>
   <si>
@@ -361,54 +355,9 @@
     <t>Escrito en Java</t>
   </si>
   <si>
-    <t>Puede ser desplegado en Glassfish 3.1.1</t>
-  </si>
-  <si>
-    <t>Puede utilizar SQL Server</t>
-  </si>
-  <si>
-    <t>Permite generación de solicitudes</t>
-  </si>
-  <si>
-    <t>Genera numero de consulta para el seguimiento de la solicitud</t>
-  </si>
-  <si>
-    <t>Permite la subdivision por areas</t>
-  </si>
-  <si>
-    <t>Es posible integrarlo con el sistema de autenticacion SSO de la universidad.</t>
-  </si>
-  <si>
-    <t>El solicitante puede ver un historial de sus solicitudes</t>
-  </si>
-  <si>
-    <t>Permite la reasignación de tareas a otras areas.</t>
-  </si>
-  <si>
-    <t>Soporta el manejo de roles</t>
-  </si>
-  <si>
-    <t>Existe la posibilidade de priorisar tareas</t>
-  </si>
-  <si>
-    <t>Existe la posibilidad de establecer fecha de termino de las tareas.</t>
-  </si>
-  <si>
-    <t>Se generan alarmas para las tareas atrasadas.</t>
-  </si>
-  <si>
-    <t>Se puede modificar el estado de las solicitudes, entre Asignada, Pendiente, En ejecucion o Finalizada (o equivalentes)</t>
-  </si>
-  <si>
-    <t>Se puede enviar notificacion por correo electronico de la finalizacion de una tarea.</t>
-  </si>
-  <si>
     <t>Version Gratuita</t>
   </si>
   <si>
-    <t>Version de Pago</t>
-  </si>
-  <si>
     <t>SI</t>
   </si>
   <si>
@@ -418,80 +367,135 @@
     <t>NO (PHP)</t>
   </si>
   <si>
-    <t>NO (MySQL)</t>
-  </si>
-  <si>
-    <r>
-      <t>Username: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color rgb="FF4A5571"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-      </rPr>
-      <t>Administrator</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Password: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color rgb="FF4A5571"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-      </rPr>
-      <t>admin</t>
-    </r>
-  </si>
-  <si>
-    <t>Envia numero de solicitud de consulta por email</t>
-  </si>
-  <si>
-    <t>Automaticamente NO, debe pedirse el envio indicando que ha olvidado el numero</t>
-  </si>
-  <si>
-    <t>Lo mas similar es dividir en categorias</t>
-  </si>
-  <si>
-    <t>Permite mover tareas a otra categoria</t>
-  </si>
-  <si>
-    <t>Soporta manejo de permisos</t>
-  </si>
-  <si>
-    <t>Se puede asignar responsables a las tareas</t>
-  </si>
-  <si>
-    <t>Se pueden ver estadisticas de las actividades que se encuentra realizando cada persona.</t>
-  </si>
-  <si>
-    <t>Solo administrador y solo ve asignadas y respondidas (no de en ejecucion ni pendientes, ni el detalle de cuales son</t>
-  </si>
-  <si>
-    <t>Lenguaje español</t>
-  </si>
-  <si>
-    <t>Ingles por defecto (Español es necesario descargarlo aparte y solo esta disponible asta la version 2.1)</t>
-  </si>
-  <si>
-    <t>SI (complicado)</t>
-  </si>
-  <si>
-    <t>Existe un perfil encargado de recibir las tareas del area y asignarles responsables</t>
+    <t>Lenguaje Español</t>
+  </si>
+  <si>
+    <t>Necesario Instalar</t>
+  </si>
+  <si>
+    <t>Idioma (por defecto)</t>
+  </si>
+  <si>
+    <t>Ingles</t>
+  </si>
+  <si>
+    <t>Base de Datos que soporta</t>
+  </si>
+  <si>
+    <t>MySQL</t>
+  </si>
+  <si>
+    <t>Servidor Web</t>
+  </si>
+  <si>
+    <t>Apache</t>
+  </si>
+  <si>
+    <t>Soporta autenticación por SSO</t>
+  </si>
+  <si>
+    <t>Permita crear diferentes areas a las que enviar las solicitudes</t>
+  </si>
+  <si>
+    <t>SI (Usa categorias)</t>
+  </si>
+  <si>
+    <t>SI (Usa Departamentos y Topicos de ayuda)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manejo de Perfiles Jerarquicos </t>
+  </si>
+  <si>
+    <t>Permite al solicitante ver su historial</t>
+  </si>
+  <si>
+    <t>Existe un perfil que pueda asignar tareas a su area.</t>
+  </si>
+  <si>
+    <t>Necesario modificar el core</t>
+  </si>
+  <si>
+    <t>Existe un perfil que pueda transferir tareas a otras areas</t>
+  </si>
+  <si>
+    <t>SI (Cualquiera puede asignar a cualquiera)</t>
+  </si>
+  <si>
+    <t>NO (Solo permisos)</t>
+  </si>
+  <si>
+    <t>Se pueden priorizar tareas</t>
+  </si>
+  <si>
+    <t>Se pueden establecer fecha maxima de termino a las tareas</t>
+  </si>
+  <si>
+    <t>Genera alarmas para tareas atrasadas</t>
+  </si>
+  <si>
+    <t>Las tareas tiene estados asignada, en espera, en desarrollo, finalizada (o similares)</t>
+  </si>
+  <si>
+    <t>NO (Lo mas similar es atraves de busquedas)</t>
+  </si>
+  <si>
+    <t>Existe visibilidad solo de las tareas del area (o grupo) excluyendo busquedas por Nº de consulta</t>
+  </si>
+  <si>
+    <t>Se puede enviar correo de notificacion al finalizar tareas</t>
+  </si>
+  <si>
+    <t>Existe perfil que vea estadisticas de las tareas de cada miembro del area</t>
+  </si>
+  <si>
+    <t>Genera y Envia Nº de Consulta para el seguimiento de la solicitud al mail</t>
+  </si>
+  <si>
+    <t>Herramientas HelpDesk</t>
+  </si>
+  <si>
+    <t>Herrmienta</t>
+  </si>
+  <si>
+    <t>SVN</t>
+  </si>
+  <si>
+    <t>Mercurial</t>
+  </si>
+  <si>
+    <t>Git</t>
+  </si>
+  <si>
+    <t>Plastic SCM</t>
+  </si>
+  <si>
+    <t>Es un sistema de control de versiones distribuido propietario desarollado en .NET por la empresa española Codice Software, sus puntos fuertes son la creacion de ramas y la replicacion de informacion entre repositorios remotos</t>
+  </si>
+  <si>
+    <t>SVN o Subversion es un sistema de control de versiones centralizado libre y de codigo fuente abierto. Permite manejar ficheros y directorios a traves del tiempo utilizando un arbol de ficheros en un repositorio central, el cual recuerda todos los cambios hechos a sus ficheros y diretorios, permitiendo asi recuperar versiones antiguas de sus datos, o examinar el historial de cambios de los mismos.     Subversion puede acceder al repositorio a traves de redes, lo que permite que varias personas puedan modificar y administrar el mismo conjunto de datos desde sus respectivas ubicaciones. Todo esto ademas permite realizar cambios sin temer que la calidad del codigo se vea afectada, ya que aunte cualquier problema se puede volver a la version anterior.</t>
+  </si>
+  <si>
+    <t>Mercurial es una herramienta libre para administracion del control de versiones. Ofrece el poder de manejar de manera eficiente sus proyectos de cualquier tamaño mientras usa una intuitiva interface. Es facil de usar y dificil de romper, haciendolo ideal para trabajar con cualquier archivo de versionados.</t>
+  </si>
+  <si>
+    <t>Git es un sistema distribuido de control de versiones libre y open sources, creado por Linus Torvalds (el creador del nucleo linux). Esta enfocado a la velocidad uso practico y manejo de proyectos grandes. Y no depende de acceso a la red o a un repositorio central, dado que al cer distribuido cada participante cuenta con una copia completa del repositorio de manera local, lo que permite trabajar sin conexion a internet.</t>
+  </si>
+  <si>
+    <t>HESK es un sistema gratuito, programado en php con mysql, que permite gestionar los tickets enviados por los clientes para poder tener organizadas todas las solicitaciones de nuevas funcionalidades o problemas detectados en nuestros productos o servicios. La versión gratuita es completamente funcional, aunque incluye algunas referencias a hesk.com.                                     Entre sus características tenemos:
+- Fácil administración, con posibilidad de tener más de un responsable por los tickets recibidos.
+- Ilimitadas categorías
+- Posibilidad de adjuntar archivos en los tickets
+- Sistema de anti-spam
+- Campos personalizados
+- Traducción sencilla a varios idiomas
+- Alertas por email</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -555,19 +559,10 @@
     </font>
     <font>
       <sz val="9"/>
-      <color rgb="FF4A5571"/>
       <name val="Verdana"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color rgb="FF4A5571"/>
-      <name val="Verdana"/>
-      <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -586,8 +581,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -597,38 +604,38 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -636,20 +643,20 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
@@ -658,41 +665,54 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="10">
+  <cellStyleXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -703,8 +723,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -763,6 +795,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="9"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -790,38 +824,44 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="9"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="10">
+  <cellStyles count="22">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="5" builtinId="8" hidden="1"/>
@@ -831,6 +871,18 @@
     <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="21" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1167,25 +1219,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D48"/>
   <sheetViews>
-    <sheetView topLeftCell="B19" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="5.5" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="3.875" customWidth="1"/>
-    <col min="3" max="3" width="66.75" customWidth="1"/>
-    <col min="4" max="4" width="5.75" style="8" customWidth="1"/>
+    <col min="2" max="2" width="3.83203125" customWidth="1"/>
+    <col min="3" max="3" width="66.6640625" customWidth="1"/>
+    <col min="4" max="4" width="5.6640625" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:4" ht="18.75">
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="2"/>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4">
       <c r="B4" s="7" t="s">
         <v>2</v>
       </c>
@@ -1196,7 +1248,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="2:4" s="1" customFormat="1" ht="42.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" s="1" customFormat="1" ht="43" customHeight="1">
       <c r="B5" s="15">
         <v>1</v>
       </c>
@@ -1207,7 +1259,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="2:4" s="1" customFormat="1" ht="42.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4" s="1" customFormat="1" ht="43" customHeight="1">
       <c r="B6" s="15">
         <v>2</v>
       </c>
@@ -1218,7 +1270,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="2:4" s="1" customFormat="1" ht="42.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" s="1" customFormat="1" ht="43" customHeight="1">
       <c r="B7" s="15">
         <v>3</v>
       </c>
@@ -1229,7 +1281,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="2:4" s="1" customFormat="1" ht="42.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:4" s="1" customFormat="1" ht="43" customHeight="1">
       <c r="B8" s="15">
         <v>4</v>
       </c>
@@ -1240,7 +1292,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="2:4" s="1" customFormat="1" ht="42.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:4" s="1" customFormat="1" ht="43" customHeight="1">
       <c r="B9" s="15">
         <v>5</v>
       </c>
@@ -1251,7 +1303,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="2:4" s="1" customFormat="1" ht="42.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:4" s="1" customFormat="1" ht="43" customHeight="1">
       <c r="B10" s="15">
         <v>6</v>
       </c>
@@ -1262,7 +1314,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="2:4" s="1" customFormat="1" ht="42.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:4" s="1" customFormat="1" ht="43" customHeight="1">
       <c r="B11" s="15">
         <v>7</v>
       </c>
@@ -1273,7 +1325,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="12" spans="2:4" s="1" customFormat="1" ht="42.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:4" s="1" customFormat="1" ht="43" customHeight="1">
       <c r="B12" s="15">
         <v>8</v>
       </c>
@@ -1284,7 +1336,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="2:4" s="1" customFormat="1" ht="42.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:4" s="1" customFormat="1" ht="43" customHeight="1">
       <c r="B13" s="15">
         <v>9</v>
       </c>
@@ -1295,7 +1347,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="2:4" ht="42.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:4" ht="43" customHeight="1">
       <c r="B14" s="15">
         <v>10</v>
       </c>
@@ -1306,7 +1358,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="2:4" ht="42.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:4" ht="43" customHeight="1">
       <c r="B15" s="15">
         <v>11</v>
       </c>
@@ -1317,7 +1369,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="16" spans="2:4" ht="42.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:4" ht="43" customHeight="1">
       <c r="B16" s="15">
         <v>12</v>
       </c>
@@ -1328,7 +1380,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="17" spans="2:4" ht="42.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:4" ht="43" customHeight="1">
       <c r="B17" s="15">
         <v>13</v>
       </c>
@@ -1339,7 +1391,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="2:4" ht="42.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4" ht="43" customHeight="1">
       <c r="B18" s="15">
         <v>14</v>
       </c>
@@ -1350,7 +1402,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="19" spans="2:4" ht="42.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:4" ht="43" customHeight="1">
       <c r="B19" s="15">
         <v>15</v>
       </c>
@@ -1361,7 +1413,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="2:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:4" ht="48.75" customHeight="1">
       <c r="B20" s="15">
         <v>16</v>
       </c>
@@ -1372,7 +1424,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="2:4" ht="42.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:4" ht="43" customHeight="1">
       <c r="B21" s="15">
         <v>17</v>
       </c>
@@ -1383,7 +1435,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="22" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:4" ht="46.5" customHeight="1">
       <c r="B22" s="15">
         <v>18</v>
       </c>
@@ -1394,7 +1446,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="23" spans="2:4" ht="42.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" ht="43" customHeight="1">
       <c r="B23" s="15">
         <v>19</v>
       </c>
@@ -1405,7 +1457,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="24" spans="2:4" ht="42.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:4" ht="43" customHeight="1">
       <c r="B24" s="15">
         <v>20</v>
       </c>
@@ -1416,7 +1468,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="25" spans="2:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:4" ht="47.25" customHeight="1">
       <c r="B25" s="15">
         <v>21</v>
       </c>
@@ -1427,57 +1479,57 @@
         <v>59</v>
       </c>
     </row>
-    <row r="26" spans="2:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="22">
+    <row r="26" spans="2:4" ht="32.25" customHeight="1">
+      <c r="B26" s="24">
         <v>22</v>
       </c>
       <c r="C26" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="D26" s="28" t="s">
+      <c r="D26" s="30" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="27" spans="2:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="23"/>
+    <row r="27" spans="2:4" ht="31.5" customHeight="1">
+      <c r="B27" s="25"/>
       <c r="C27" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="D27" s="29"/>
-    </row>
-    <row r="28" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="24"/>
+      <c r="D27" s="31"/>
+    </row>
+    <row r="28" spans="2:4" ht="46.5" customHeight="1">
+      <c r="B28" s="26"/>
       <c r="C28" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="D28" s="30"/>
-    </row>
-    <row r="29" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="25">
+      <c r="D28" s="32"/>
+    </row>
+    <row r="29" spans="2:4" ht="29.25" customHeight="1">
+      <c r="B29" s="27">
         <v>23</v>
       </c>
       <c r="C29" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="D29" s="28" t="s">
+      <c r="D29" s="30" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="30" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="26"/>
+    <row r="30" spans="2:4" ht="30" customHeight="1">
+      <c r="B30" s="28"/>
       <c r="C30" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="D30" s="29"/>
-    </row>
-    <row r="31" spans="2:4" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="27"/>
+      <c r="D30" s="31"/>
+    </row>
+    <row r="31" spans="2:4" ht="39" customHeight="1">
+      <c r="B31" s="29"/>
       <c r="C31" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="D31" s="30"/>
-    </row>
-    <row r="32" spans="2:4" ht="42.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D31" s="32"/>
+    </row>
+    <row r="32" spans="2:4" ht="43" customHeight="1">
       <c r="B32" s="15">
         <v>24</v>
       </c>
@@ -1488,7 +1540,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="33" spans="2:4" ht="42.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:4" ht="43" customHeight="1">
       <c r="B33" s="15">
         <v>25</v>
       </c>
@@ -1499,7 +1551,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="34" spans="2:4" ht="42.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:4" ht="43" customHeight="1">
       <c r="B34" s="15">
         <v>26</v>
       </c>
@@ -1510,7 +1562,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="35" spans="2:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:4" ht="45" customHeight="1">
       <c r="B35" s="15">
         <v>27</v>
       </c>
@@ -1521,7 +1573,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="36" spans="2:4" ht="42.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:4" ht="43" customHeight="1">
       <c r="B36" s="15">
         <v>28</v>
       </c>
@@ -1532,7 +1584,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="37" spans="2:4" ht="42.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:4" ht="43" customHeight="1">
       <c r="B37" s="15">
         <v>29</v>
       </c>
@@ -1543,7 +1595,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="38" spans="2:4" ht="42.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:4" ht="43" customHeight="1">
       <c r="B38" s="15">
         <v>30</v>
       </c>
@@ -1554,7 +1606,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="39" spans="2:4" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:4" ht="45.75" customHeight="1">
       <c r="B39" s="15">
         <v>31</v>
       </c>
@@ -1565,7 +1617,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="40" spans="2:4" ht="42.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:4" ht="43" customHeight="1">
       <c r="B40" s="15">
         <v>32</v>
       </c>
@@ -1576,7 +1628,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="41" spans="2:4" ht="42.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:4" ht="43" customHeight="1">
       <c r="B41" s="15">
         <v>33</v>
       </c>
@@ -1587,7 +1639,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="42" spans="2:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:4" ht="47.25" customHeight="1">
       <c r="B42" s="15">
         <v>34</v>
       </c>
@@ -1598,7 +1650,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="43" spans="2:4" ht="42.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:4" ht="43" customHeight="1">
       <c r="B43" s="15">
         <v>35</v>
       </c>
@@ -1609,7 +1661,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="44" spans="2:4" ht="42.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:4" ht="43" customHeight="1">
       <c r="B44" s="15">
         <v>36</v>
       </c>
@@ -1620,7 +1672,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="45" spans="2:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:4" ht="47.25" customHeight="1">
       <c r="B45" s="15">
         <v>37</v>
       </c>
@@ -1631,7 +1683,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="46" spans="2:4" ht="42.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:4" ht="43" customHeight="1">
       <c r="B46" s="15">
         <v>38</v>
       </c>
@@ -1642,7 +1694,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="47" spans="2:4" ht="42.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:4" ht="43" customHeight="1">
       <c r="B47" s="15">
         <v>39</v>
       </c>
@@ -1653,7 +1705,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="48" spans="2:4" ht="42.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:4" ht="43" customHeight="1">
       <c r="B48" s="15">
         <v>40</v>
       </c>
@@ -1672,7 +1724,7 @@
     <mergeCell ref="D29:D31"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1685,24 +1737,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D20"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="4.25" customWidth="1"/>
-    <col min="2" max="2" width="6.875" customWidth="1"/>
-    <col min="3" max="3" width="66.25" customWidth="1"/>
+    <col min="1" max="1" width="4.1640625" customWidth="1"/>
+    <col min="2" max="2" width="6.83203125" customWidth="1"/>
+    <col min="3" max="3" width="66.1640625" customWidth="1"/>
     <col min="4" max="4" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:4" ht="18.75">
       <c r="B2" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4">
       <c r="B4" s="7" t="s">
         <v>2</v>
       </c>
@@ -1713,7 +1765,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="2:4" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" ht="40" customHeight="1">
       <c r="B5" s="9">
         <v>1</v>
       </c>
@@ -1722,7 +1774,7 @@
       </c>
       <c r="D5" s="3"/>
     </row>
-    <row r="6" spans="2:4" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4" ht="40" customHeight="1">
       <c r="B6" s="9">
         <v>2</v>
       </c>
@@ -1731,7 +1783,7 @@
       </c>
       <c r="D6" s="3"/>
     </row>
-    <row r="7" spans="2:4" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" ht="40" customHeight="1">
       <c r="B7" s="9">
         <v>3</v>
       </c>
@@ -1740,7 +1792,7 @@
       </c>
       <c r="D7" s="3"/>
     </row>
-    <row r="8" spans="2:4" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:4" ht="40" customHeight="1">
       <c r="B8" s="9">
         <v>4</v>
       </c>
@@ -1749,7 +1801,7 @@
       </c>
       <c r="D8" s="3"/>
     </row>
-    <row r="9" spans="2:4" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:4" ht="40" customHeight="1">
       <c r="B9" s="9">
         <v>5</v>
       </c>
@@ -1758,7 +1810,7 @@
       </c>
       <c r="D9" s="3"/>
     </row>
-    <row r="10" spans="2:4" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:4" ht="40" customHeight="1">
       <c r="B10" s="9">
         <v>6</v>
       </c>
@@ -1769,61 +1821,61 @@
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="2:4" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:4" ht="40" customHeight="1">
       <c r="B11" s="9">
         <v>7</v>
       </c>
       <c r="C11" s="10"/>
     </row>
-    <row r="12" spans="2:4" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:4" ht="40" customHeight="1">
       <c r="B12" s="9">
         <v>8</v>
       </c>
       <c r="C12" s="10"/>
     </row>
-    <row r="13" spans="2:4" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:4" ht="40" customHeight="1">
       <c r="B13" s="9">
         <v>9</v>
       </c>
       <c r="C13" s="10"/>
     </row>
-    <row r="14" spans="2:4" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:4" ht="40" customHeight="1">
       <c r="B14" s="9">
         <v>10</v>
       </c>
       <c r="C14" s="10"/>
     </row>
-    <row r="15" spans="2:4" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:4" ht="40" customHeight="1">
       <c r="B15" s="9">
         <v>11</v>
       </c>
       <c r="C15" s="10"/>
     </row>
-    <row r="16" spans="2:4" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:4" ht="40" customHeight="1">
       <c r="B16" s="9">
         <v>12</v>
       </c>
       <c r="C16" s="10"/>
     </row>
-    <row r="17" spans="2:3" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:3" ht="40" customHeight="1">
       <c r="B17" s="9">
         <v>13</v>
       </c>
       <c r="C17" s="10"/>
     </row>
-    <row r="18" spans="2:3" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:3" ht="40" customHeight="1">
       <c r="B18" s="9">
         <v>14</v>
       </c>
       <c r="C18" s="10"/>
     </row>
-    <row r="19" spans="2:3" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:3" ht="40" customHeight="1">
       <c r="B19" s="9">
         <v>15</v>
       </c>
       <c r="C19" s="10"/>
     </row>
-    <row r="20" spans="2:3" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:3" ht="40" customHeight="1">
       <c r="B20" s="9">
         <v>16</v>
       </c>
@@ -1831,6 +1883,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1842,18 +1899,18 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="19.25" customWidth="1"/>
-    <col min="3" max="3" width="61.125" customWidth="1"/>
+    <col min="2" max="2" width="19.1640625" customWidth="1"/>
+    <col min="3" max="3" width="61.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:3">
       <c r="B2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="2:3" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3" s="12" customFormat="1" ht="30" customHeight="1">
       <c r="B4" s="13" t="s">
         <v>18</v>
       </c>
@@ -1861,7 +1918,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="2:3" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:3" s="12" customFormat="1" ht="30" customHeight="1">
       <c r="B5" s="13" t="s">
         <v>6</v>
       </c>
@@ -1869,7 +1926,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="2:3" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:3" s="12" customFormat="1" ht="30" customHeight="1">
       <c r="B6" s="13" t="s">
         <v>17</v>
       </c>
@@ -1877,13 +1934,13 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="2:3" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:3" s="12" customFormat="1" ht="30" customHeight="1">
       <c r="B7" s="13" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="5"/>
     </row>
-    <row r="8" spans="2:3" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:3" s="12" customFormat="1" ht="30" customHeight="1">
       <c r="B8" s="13" t="s">
         <v>8</v>
       </c>
@@ -1891,7 +1948,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="2:3" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:3" s="12" customFormat="1" ht="30" customHeight="1">
       <c r="B9" s="13" t="s">
         <v>11</v>
       </c>
@@ -1899,7 +1956,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:3">
       <c r="B10" s="21" t="s">
         <v>69</v>
       </c>
@@ -1907,7 +1964,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:3">
       <c r="B11" s="21" t="s">
         <v>70</v>
       </c>
@@ -1915,9 +1972,9 @@
         <v>71</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B13" s="34" t="s">
-        <v>83</v>
+    <row r="13" spans="2:3">
+      <c r="B13" s="23" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -1932,27 +1989,27 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D5"/>
+  <dimension ref="B2:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="3.125" customWidth="1"/>
-    <col min="2" max="2" width="14.875" customWidth="1"/>
+    <col min="1" max="1" width="3.1640625" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" customWidth="1"/>
     <col min="3" max="3" width="28.5" customWidth="1"/>
-    <col min="4" max="4" width="31.625" customWidth="1"/>
+    <col min="4" max="4" width="31.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="2:4" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4" ht="22.5" customHeight="1"/>
+    <row r="4" spans="2:4" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="B4" s="5" t="s">
         <v>76</v>
       </c>
@@ -1963,12 +2020,17 @@
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4">
       <c r="B5" t="s">
-        <v>80</v>
-      </c>
-      <c r="D5" s="31" t="s">
         <v>79</v>
+      </c>
+      <c r="D5" s="22" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4">
+      <c r="B8" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -1976,7 +2038,7 @@
     <hyperlink ref="D5" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1987,352 +2049,357 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:F36"/>
+  <dimension ref="B2:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="8.25" customWidth="1"/>
-    <col min="2" max="2" width="32.625" customWidth="1"/>
-    <col min="3" max="3" width="32.75" style="32" customWidth="1"/>
-    <col min="4" max="4" width="11" style="32"/>
+    <col min="1" max="1" width="4.6640625" customWidth="1"/>
+    <col min="2" max="2" width="23.6640625" customWidth="1"/>
+    <col min="3" max="3" width="21.33203125" style="8" customWidth="1"/>
+    <col min="4" max="4" width="22.5" style="8" customWidth="1"/>
+    <col min="5" max="5" width="37.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C3" s="33" t="s">
-        <v>81</v>
-      </c>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C4" s="42" t="s">
+    <row r="2" spans="2:4">
+      <c r="C2" s="39" t="s">
+        <v>115</v>
+      </c>
+      <c r="D2" s="40"/>
+    </row>
+    <row r="3" spans="2:4">
+      <c r="C3" s="34" t="s">
+        <v>79</v>
+      </c>
+      <c r="D3" s="34" t="s">
         <v>80</v>
       </c>
-      <c r="D4" s="42" t="s">
+    </row>
+    <row r="4" spans="2:4" s="33" customFormat="1">
+      <c r="B4" s="36" t="s">
+        <v>83</v>
+      </c>
+      <c r="C4" s="35" t="s">
+        <v>84</v>
+      </c>
+      <c r="D4" s="35" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" s="33" customFormat="1">
+      <c r="B5" s="36" t="s">
+        <v>89</v>
+      </c>
+      <c r="C5" s="35" t="s">
+        <v>90</v>
+      </c>
+      <c r="D5" s="35" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" s="33" customFormat="1" ht="30">
+      <c r="B6" s="37" t="s">
+        <v>87</v>
+      </c>
+      <c r="C6" s="35" t="s">
+        <v>88</v>
+      </c>
+      <c r="D6" s="35" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" s="33" customFormat="1">
+      <c r="B7" s="36" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="5" spans="2:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="39" t="s">
+      <c r="C7" s="35" t="s">
+        <v>86</v>
+      </c>
+      <c r="D7" s="35" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" s="33" customFormat="1">
+      <c r="B8" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="C8" s="35" t="s">
+        <v>92</v>
+      </c>
+      <c r="D8" s="35" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" s="33" customFormat="1">
+      <c r="B9" s="36" t="s">
+        <v>93</v>
+      </c>
+      <c r="C9" s="35" t="s">
+        <v>94</v>
+      </c>
+      <c r="D9" s="35" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" s="33" customFormat="1" ht="25">
+      <c r="B10" s="36" t="s">
+        <v>95</v>
+      </c>
+      <c r="C10" s="35" t="s">
+        <v>85</v>
+      </c>
+      <c r="D10" s="35" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" ht="37">
+      <c r="B11" s="36" t="s">
+        <v>114</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" ht="37">
+      <c r="B12" s="36" t="s">
+        <v>96</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" ht="25">
+      <c r="B13" s="36" t="s">
         <v>99</v>
       </c>
-      <c r="C5" s="36" t="s">
+      <c r="C13" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" ht="25">
+      <c r="B14" s="36" t="s">
+        <v>100</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" ht="30">
+      <c r="B15" s="36" t="s">
         <v>101</v>
       </c>
-      <c r="D5" s="36" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="39" t="s">
-        <v>100</v>
-      </c>
-      <c r="C6" s="36" t="s">
-        <v>101</v>
-      </c>
-      <c r="D6" s="36"/>
-    </row>
-    <row r="7" spans="2:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="39" t="s">
-        <v>78</v>
-      </c>
-      <c r="C7" s="36" t="s">
-        <v>101</v>
-      </c>
-      <c r="D7" s="36"/>
-    </row>
-    <row r="8" spans="2:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="39" t="s">
+      <c r="C15" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" ht="31" customHeight="1">
+      <c r="B16" s="37" t="s">
+        <v>103</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="D16" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="C8" s="36" t="s">
-        <v>103</v>
-      </c>
-      <c r="D8" s="36" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" s="12" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B9" s="39" t="s">
-        <v>115</v>
-      </c>
-      <c r="C9" s="36" t="s">
-        <v>116</v>
-      </c>
-      <c r="D9" s="36" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="39"/>
-      <c r="C10" s="36"/>
-      <c r="D10" s="36"/>
-    </row>
-    <row r="11" spans="2:6" s="12" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B11" s="39" t="s">
+    </row>
+    <row r="17" spans="2:5">
+      <c r="B17" s="36" t="s">
+        <v>106</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="37">
+      <c r="B18" s="36" t="s">
+        <v>107</v>
+      </c>
+      <c r="C18" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="C11" s="36" t="s">
-        <v>102</v>
-      </c>
-      <c r="D11" s="36" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="39" t="s">
-        <v>86</v>
-      </c>
-      <c r="C12" s="36" t="s">
-        <v>104</v>
-      </c>
-      <c r="D12" s="36" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="39" t="s">
-        <v>87</v>
-      </c>
-      <c r="C13" s="36" t="s">
-        <v>101</v>
-      </c>
-      <c r="D13" s="36" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" s="12" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B14" s="39" t="s">
-        <v>88</v>
-      </c>
-      <c r="C14" s="36" t="s">
-        <v>101</v>
-      </c>
-      <c r="D14" s="36" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" s="12" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B15" s="39" t="s">
-        <v>107</v>
-      </c>
-      <c r="C15" s="36" t="s">
+      <c r="D18" s="9" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" ht="25">
+      <c r="B19" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="D15" s="36" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="39" t="s">
-        <v>89</v>
-      </c>
-      <c r="C16" s="36" t="s">
+      <c r="C19" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" ht="49">
+      <c r="B20" s="36" t="s">
         <v>109</v>
       </c>
-      <c r="D16" s="36" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" s="12" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="39" t="s">
-        <v>90</v>
-      </c>
-      <c r="C17" s="36" t="s">
-        <v>102</v>
-      </c>
-      <c r="D17" s="36" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" s="12" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B18" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="C18" s="36" t="s">
-        <v>102</v>
-      </c>
-      <c r="D18" s="36" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" s="12" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B19" s="40" t="s">
-        <v>92</v>
-      </c>
-      <c r="C19" s="36" t="s">
+      <c r="C20" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" ht="37">
+      <c r="B21" s="36" t="s">
+        <v>113</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="D21" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="D19" s="36" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="40" t="s">
-        <v>93</v>
-      </c>
-      <c r="C20" s="36" t="s">
+    </row>
+    <row r="22" spans="2:5" ht="49">
+      <c r="B22" s="36" t="s">
         <v>111</v>
       </c>
-      <c r="D20" s="36" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" s="1" customFormat="1" ht="63" x14ac:dyDescent="0.25">
-      <c r="B21" s="39" t="s">
-        <v>113</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" s="12" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B22" s="40" t="s">
-        <v>94</v>
-      </c>
-      <c r="C22" s="36" t="s">
-        <v>101</v>
-      </c>
-      <c r="D22" s="36" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" s="12" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B23" s="40" t="s">
-        <v>95</v>
-      </c>
-      <c r="C23" s="36" t="s">
-        <v>102</v>
-      </c>
-      <c r="D23" s="36"/>
-    </row>
-    <row r="24" spans="2:4" s="12" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B24" s="40" t="s">
-        <v>96</v>
-      </c>
-      <c r="C24" s="36" t="s">
-        <v>102</v>
-      </c>
-      <c r="D24" s="36"/>
-    </row>
-    <row r="25" spans="2:4" s="12" customFormat="1" ht="63" x14ac:dyDescent="0.25">
-      <c r="B25" s="40" t="s">
-        <v>97</v>
-      </c>
-      <c r="C25" s="36" t="s">
-        <v>101</v>
-      </c>
-      <c r="D25" s="36" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="26" spans="2:4" s="12" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B26" s="40" t="s">
-        <v>98</v>
-      </c>
-      <c r="C26" s="36" t="s">
-        <v>102</v>
-      </c>
-      <c r="D26" s="36" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="27" spans="2:4" s="12" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B27" s="41" t="s">
+      <c r="C22" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" ht="25">
+      <c r="B23" s="36" t="s">
         <v>112</v>
       </c>
-      <c r="C27" s="36" t="s">
-        <v>102</v>
-      </c>
-      <c r="D27" s="36" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="28" spans="2:4" s="12" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B28" s="35" t="s">
-        <v>118</v>
-      </c>
-      <c r="C28" s="36" t="s">
-        <v>102</v>
-      </c>
-      <c r="D28" s="36" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="29" spans="2:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C29" s="37"/>
-      <c r="D29" s="37"/>
-    </row>
-    <row r="30" spans="2:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C30" s="37"/>
-      <c r="D30" s="37"/>
-    </row>
-    <row r="31" spans="2:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C31" s="37"/>
-      <c r="D31" s="37"/>
-    </row>
-    <row r="32" spans="2:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C32" s="37"/>
-      <c r="D32" s="37"/>
-    </row>
-    <row r="33" spans="3:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C33" s="37"/>
-      <c r="D33" s="37"/>
-    </row>
-    <row r="34" spans="3:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C34" s="37"/>
-      <c r="D34" s="37"/>
-    </row>
-    <row r="35" spans="3:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C35" s="37"/>
-      <c r="D35" s="37"/>
-    </row>
-    <row r="36" spans="3:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C36" s="37"/>
-      <c r="D36" s="37"/>
+      <c r="C23" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" ht="102" customHeight="1">
+      <c r="B28" s="38" t="s">
+        <v>79</v>
+      </c>
+      <c r="C28" s="44" t="s">
+        <v>125</v>
+      </c>
+      <c r="D28" s="44"/>
+      <c r="E28" s="44"/>
+    </row>
+    <row r="29" spans="2:5" ht="137" customHeight="1">
+      <c r="B29" s="38"/>
+      <c r="C29" s="44"/>
+      <c r="D29" s="44"/>
+      <c r="E29" s="44"/>
+    </row>
+    <row r="30" spans="2:5" ht="32" customHeight="1">
+      <c r="B30" s="38" t="s">
+        <v>80</v>
+      </c>
+      <c r="C30" s="38"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="38"/>
+    </row>
+    <row r="31" spans="2:5" ht="33" customHeight="1">
+      <c r="B31" s="38"/>
+      <c r="C31" s="38"/>
+      <c r="D31" s="38"/>
+      <c r="E31" s="38"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="C3:F3"/>
+  <mergeCells count="5">
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="C28:E29"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="C30:E31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:B5"/>
+  <dimension ref="B3:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView topLeftCell="A4" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="3.1640625" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" customWidth="1"/>
+    <col min="3" max="3" width="82.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B4" s="38" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B5" s="38" t="s">
-        <v>106</v>
+    <row r="3" spans="2:3" s="41" customFormat="1" ht="140" customHeight="1">
+      <c r="B3" s="42" t="s">
+        <v>117</v>
+      </c>
+      <c r="C3" s="43" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" s="41" customFormat="1" ht="71" customHeight="1">
+      <c r="B4" s="42" t="s">
+        <v>118</v>
+      </c>
+      <c r="C4" s="43" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" s="41" customFormat="1" ht="89" customHeight="1">
+      <c r="B5" s="42" t="s">
+        <v>119</v>
+      </c>
+      <c r="C5" s="43" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" s="41" customFormat="1" ht="71" customHeight="1">
+      <c r="B6" s="42" t="s">
+        <v>120</v>
+      </c>
+      <c r="C6" s="43" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se agregan al excel modificaciones pendientes a realizar en el proyecto
</commit_message>
<xml_diff>
--- a/Informes/Requerimientos.xlsx
+++ b/Informes/Requerimientos.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22220"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14720" tabRatio="602" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14720" tabRatio="602" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Req. F" sheetId="2" r:id="rId1"/>
@@ -13,6 +13,7 @@
     <sheet name="Herramientas" sheetId="1" r:id="rId4"/>
     <sheet name="Evaluacion Herramienta HelpDesk" sheetId="6" r:id="rId5"/>
     <sheet name="Evaluacion Herramienta SCM" sheetId="7" r:id="rId6"/>
+    <sheet name="Casos de Uso" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="140000" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="166">
   <si>
     <t>Herramientas para la Asignación de Tareas</t>
   </si>
@@ -489,6 +490,126 @@
 - Campos personalizados
 - Traducción sencilla a varios idiomas
 - Alertas por email</t>
+  </si>
+  <si>
+    <t>Caso de Uso</t>
+  </si>
+  <si>
+    <t>Crear Solicitud</t>
+  </si>
+  <si>
+    <t>Consultar Solicitud</t>
+  </si>
+  <si>
+    <t>Enviar Numero de Consulta</t>
+  </si>
+  <si>
+    <t>Respuesta Manual</t>
+  </si>
+  <si>
+    <t>Enviar Email</t>
+  </si>
+  <si>
+    <t>Gestionar Solicitud</t>
+  </si>
+  <si>
+    <t>Comentar Solicitud</t>
+  </si>
+  <si>
+    <t>Eliminar</t>
+  </si>
+  <si>
+    <t>Convertir en Proyecto</t>
+  </si>
+  <si>
+    <t>Responder Solicitud</t>
+  </si>
+  <si>
+    <t>Transferir Solicitud</t>
+  </si>
+  <si>
+    <t>Rechazar Solicitud</t>
+  </si>
+  <si>
+    <t>Asignar Solicitud</t>
+  </si>
+  <si>
+    <t>Ver Resumen Area</t>
+  </si>
+  <si>
+    <t>Buscar Solicitudes</t>
+  </si>
+  <si>
+    <t>Ver Resumen Departamento</t>
+  </si>
+  <si>
+    <t>Ver Resumen Funcionario</t>
+  </si>
+  <si>
+    <t>Atender Solicitud</t>
+  </si>
+  <si>
+    <t>Iniciar Solicitud</t>
+  </si>
+  <si>
+    <t>Cerrar Solicitud</t>
+  </si>
+  <si>
+    <t>Respuesta al Jefe de Area</t>
+  </si>
+  <si>
+    <t>Respuesta al Solicitante</t>
+  </si>
+  <si>
+    <t>Gestionar Usuario</t>
+  </si>
+  <si>
+    <t>Crear Usuario</t>
+  </si>
+  <si>
+    <t>Eliminar Usuario</t>
+  </si>
+  <si>
+    <t>Asignar Permisos</t>
+  </si>
+  <si>
+    <t>Gestionar Areas</t>
+  </si>
+  <si>
+    <t>Crear Area</t>
+  </si>
+  <si>
+    <t>Editar Area</t>
+  </si>
+  <si>
+    <t>Eliminar Area</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Agregar a los Req y Cambiar Nombre a Ver Resumen Personal</t>
+  </si>
+  <si>
+    <t>Indicar Satisfacción (Cliente)</t>
+  </si>
+  <si>
+    <t>Agregar a los req y a los casos de uso</t>
+  </si>
+  <si>
+    <t>Especificar en los requerimientos cuales son los indicadores a medir</t>
+  </si>
+  <si>
+    <t>Responder al Solicitante</t>
+  </si>
+  <si>
+    <t>Cambiar a Respuesta directa en req y diagrama</t>
+  </si>
+  <si>
+    <t>Usuarios y permisos manejados por LDAP (Preguntar a gazmuri)</t>
+  </si>
+  <si>
+    <t>Eliminar Asignar Personal de los casos de uso ya q se puede considerar dentro de modificar</t>
   </si>
 </sst>
 </file>
@@ -562,7 +683,7 @@
       <name val="Verdana"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -608,6 +729,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -730,7 +857,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="22">
+  <cellStyleXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -753,8 +880,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -840,6 +970,60 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -852,62 +1036,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="22">
+  <cellStyles count="25">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="5" builtinId="8" hidden="1"/>
@@ -929,6 +1071,9 @@
     <cellStyle name="Hipervínculo visitado" xfId="19" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1277,7 +1422,7 @@
     <col min="4" max="4" width="5.6640625" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" ht="18.75">
+    <row r="2" spans="1:4" ht="18">
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1472,13 +1617,13 @@
       </c>
     </row>
     <row r="21" spans="2:4" ht="43" customHeight="1">
-      <c r="B21" s="37">
+      <c r="B21" s="33">
         <v>17</v>
       </c>
-      <c r="C21" s="38" t="s">
+      <c r="C21" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="D21" s="39" t="s">
+      <c r="D21" s="35" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1505,118 +1650,118 @@
       </c>
     </row>
     <row r="24" spans="2:4" ht="43" customHeight="1">
-      <c r="B24" s="40">
+      <c r="B24" s="36">
         <v>20</v>
       </c>
-      <c r="C24" s="41" t="s">
+      <c r="C24" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="D24" s="42" t="s">
+      <c r="D24" s="38" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="25" spans="2:4" ht="47.25" customHeight="1">
-      <c r="B25" s="40">
+      <c r="B25" s="36">
         <v>21</v>
       </c>
-      <c r="C25" s="41" t="s">
+      <c r="C25" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="D25" s="42" t="s">
+      <c r="D25" s="38" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="26" spans="2:4" ht="32.25" customHeight="1">
-      <c r="B26" s="43">
+      <c r="B26" s="42">
         <v>22</v>
       </c>
-      <c r="C26" s="44" t="s">
+      <c r="C26" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="D26" s="45" t="s">
+      <c r="D26" s="48" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="27" spans="2:4" ht="31.5" customHeight="1">
-      <c r="B27" s="46"/>
-      <c r="C27" s="47" t="s">
+      <c r="B27" s="43"/>
+      <c r="C27" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="D27" s="48"/>
+      <c r="D27" s="49"/>
     </row>
     <row r="28" spans="2:4" ht="46.5" customHeight="1">
-      <c r="B28" s="49"/>
-      <c r="C28" s="50" t="s">
+      <c r="B28" s="44"/>
+      <c r="C28" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="D28" s="51"/>
+      <c r="D28" s="50"/>
     </row>
     <row r="29" spans="2:4" ht="29.25" customHeight="1">
-      <c r="B29" s="52">
+      <c r="B29" s="45">
         <v>23</v>
       </c>
-      <c r="C29" s="44" t="s">
+      <c r="C29" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="D29" s="45" t="s">
+      <c r="D29" s="48" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="30" spans="2:4" ht="30" customHeight="1">
-      <c r="B30" s="53"/>
-      <c r="C30" s="47" t="s">
+      <c r="B30" s="46"/>
+      <c r="C30" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="D30" s="48"/>
+      <c r="D30" s="49"/>
     </row>
     <row r="31" spans="2:4" ht="39" customHeight="1">
-      <c r="B31" s="54"/>
-      <c r="C31" s="50" t="s">
+      <c r="B31" s="47"/>
+      <c r="C31" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="D31" s="51"/>
+      <c r="D31" s="50"/>
     </row>
     <row r="32" spans="2:4" ht="43" customHeight="1">
-      <c r="B32" s="40">
+      <c r="B32" s="36">
         <v>24</v>
       </c>
-      <c r="C32" s="41" t="s">
+      <c r="C32" s="37" t="s">
         <v>67</v>
       </c>
-      <c r="D32" s="42" t="s">
+      <c r="D32" s="38" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="33" spans="2:4" ht="43" customHeight="1">
-      <c r="B33" s="40">
+      <c r="B33" s="36">
         <v>25</v>
       </c>
-      <c r="C33" s="41" t="s">
+      <c r="C33" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="D33" s="42" t="s">
+      <c r="D33" s="38" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="34" spans="2:4" ht="43" customHeight="1">
-      <c r="B34" s="40">
+      <c r="B34" s="36">
         <v>26</v>
       </c>
-      <c r="C34" s="41" t="s">
+      <c r="C34" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="D34" s="42" t="s">
+      <c r="D34" s="38" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="35" spans="2:4" ht="45" customHeight="1">
-      <c r="B35" s="40">
+      <c r="B35" s="36">
         <v>27</v>
       </c>
-      <c r="C35" s="41" t="s">
+      <c r="C35" s="37" t="s">
         <v>65</v>
       </c>
-      <c r="D35" s="42" t="s">
+      <c r="D35" s="38" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1654,13 +1799,13 @@
       </c>
     </row>
     <row r="39" spans="2:4" ht="45.75" customHeight="1">
-      <c r="B39" s="40">
+      <c r="B39" s="36">
         <v>31</v>
       </c>
-      <c r="C39" s="41" t="s">
+      <c r="C39" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="D39" s="42" t="s">
+      <c r="D39" s="38" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1698,24 +1843,24 @@
       </c>
     </row>
     <row r="43" spans="2:4" ht="43" customHeight="1">
-      <c r="B43" s="40">
+      <c r="B43" s="36">
         <v>35</v>
       </c>
-      <c r="C43" s="41" t="s">
+      <c r="C43" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="D43" s="40" t="s">
+      <c r="D43" s="36" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="44" spans="2:4" ht="43" customHeight="1">
-      <c r="B44" s="40">
+      <c r="B44" s="36">
         <v>36</v>
       </c>
-      <c r="C44" s="41" t="s">
+      <c r="C44" s="37" t="s">
         <v>74</v>
       </c>
-      <c r="D44" s="42" t="s">
+      <c r="D44" s="38" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1784,7 +1929,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+    <sheetView topLeftCell="A8" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -1796,7 +1941,7 @@
     <col min="4" max="4" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" ht="18.75">
+    <row r="2" spans="2:4" ht="18">
       <c r="B2" s="2" t="s">
         <v>10</v>
       </c>
@@ -2112,10 +2257,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4">
-      <c r="C2" s="33" t="s">
+      <c r="C2" s="51" t="s">
         <v>115</v>
       </c>
-      <c r="D2" s="34"/>
+      <c r="D2" s="52"/>
     </row>
     <row r="3" spans="2:4">
       <c r="C3" s="22" t="s">
@@ -2147,7 +2292,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="2:4" s="21" customFormat="1" ht="31.5">
+    <row r="6" spans="2:4" s="21" customFormat="1" ht="30">
       <c r="B6" s="25" t="s">
         <v>87</v>
       </c>
@@ -2191,7 +2336,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="10" spans="2:4" s="21" customFormat="1" ht="24">
+    <row r="10" spans="2:4" s="21" customFormat="1" ht="25">
       <c r="B10" s="24" t="s">
         <v>95</v>
       </c>
@@ -2202,7 +2347,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="11" spans="2:4" ht="46.5">
+    <row r="11" spans="2:4" ht="37">
       <c r="B11" s="24" t="s">
         <v>114</v>
       </c>
@@ -2213,7 +2358,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="12" spans="2:4" ht="35.25">
+    <row r="12" spans="2:4" ht="37">
       <c r="B12" s="24" t="s">
         <v>96</v>
       </c>
@@ -2224,7 +2369,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="13" spans="2:4" ht="24">
+    <row r="13" spans="2:4" ht="25">
       <c r="B13" s="24" t="s">
         <v>99</v>
       </c>
@@ -2235,7 +2380,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="14" spans="2:4" ht="24">
+    <row r="14" spans="2:4" ht="25">
       <c r="B14" s="24" t="s">
         <v>100</v>
       </c>
@@ -2246,7 +2391,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="15" spans="2:4" ht="31.5">
+    <row r="15" spans="2:4" ht="30">
       <c r="B15" s="24" t="s">
         <v>101</v>
       </c>
@@ -2279,7 +2424,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="18" spans="2:5" ht="35.25">
+    <row r="18" spans="2:5" ht="37">
       <c r="B18" s="24" t="s">
         <v>107</v>
       </c>
@@ -2290,7 +2435,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="19" spans="2:5" ht="24">
+    <row r="19" spans="2:5" ht="25">
       <c r="B19" s="24" t="s">
         <v>108</v>
       </c>
@@ -2301,7 +2446,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="20" spans="2:5" ht="46.5">
+    <row r="20" spans="2:5" ht="49">
       <c r="B20" s="24" t="s">
         <v>109</v>
       </c>
@@ -2312,7 +2457,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="21" spans="2:5" ht="35.25">
+    <row r="21" spans="2:5" ht="37">
       <c r="B21" s="24" t="s">
         <v>113</v>
       </c>
@@ -2323,7 +2468,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="22" spans="2:5" ht="46.5">
+    <row r="22" spans="2:5" ht="49">
       <c r="B22" s="24" t="s">
         <v>111</v>
       </c>
@@ -2334,7 +2479,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="23" spans="2:5" ht="35.25">
+    <row r="23" spans="2:5" ht="25">
       <c r="B23" s="24" t="s">
         <v>112</v>
       </c>
@@ -2346,34 +2491,34 @@
       </c>
     </row>
     <row r="28" spans="2:5" ht="102" customHeight="1">
-      <c r="B28" s="35" t="s">
+      <c r="B28" s="53" t="s">
         <v>79</v>
       </c>
-      <c r="C28" s="36" t="s">
+      <c r="C28" s="54" t="s">
         <v>125</v>
       </c>
-      <c r="D28" s="36"/>
-      <c r="E28" s="36"/>
+      <c r="D28" s="54"/>
+      <c r="E28" s="54"/>
     </row>
     <row r="29" spans="2:5" ht="137" customHeight="1">
-      <c r="B29" s="35"/>
-      <c r="C29" s="36"/>
-      <c r="D29" s="36"/>
-      <c r="E29" s="36"/>
+      <c r="B29" s="53"/>
+      <c r="C29" s="54"/>
+      <c r="D29" s="54"/>
+      <c r="E29" s="54"/>
     </row>
     <row r="30" spans="2:5" ht="32" customHeight="1">
-      <c r="B30" s="35" t="s">
+      <c r="B30" s="53" t="s">
         <v>80</v>
       </c>
-      <c r="C30" s="35"/>
-      <c r="D30" s="35"/>
-      <c r="E30" s="35"/>
+      <c r="C30" s="53"/>
+      <c r="D30" s="53"/>
+      <c r="E30" s="53"/>
     </row>
     <row r="31" spans="2:5" ht="33" customHeight="1">
-      <c r="B31" s="35"/>
-      <c r="C31" s="35"/>
-      <c r="D31" s="35"/>
-      <c r="E31" s="35"/>
+      <c r="B31" s="53"/>
+      <c r="C31" s="53"/>
+      <c r="D31" s="53"/>
+      <c r="E31" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2449,4 +2594,292 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:D37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="38" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" style="56" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4">
+      <c r="B2" s="59" t="s">
+        <v>126</v>
+      </c>
+      <c r="C2" s="60"/>
+    </row>
+    <row r="3" spans="2:4">
+      <c r="B3" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="C3" s="57" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4">
+      <c r="B4" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C4" s="57" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4">
+      <c r="B5" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="C5" s="57" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4">
+      <c r="B6" s="58" t="s">
+        <v>133</v>
+      </c>
+      <c r="C6" s="57" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4">
+      <c r="B7" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C7" s="57" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4">
+      <c r="B8" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C8" s="57" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4">
+      <c r="B9" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="C9" s="57" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4">
+      <c r="B10" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C10" s="57" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4">
+      <c r="B11" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="C11" s="57" t="s">
+        <v>157</v>
+      </c>
+      <c r="D11" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4">
+      <c r="B12" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C12" s="57" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4">
+      <c r="B13" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C13" s="57" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4">
+      <c r="B14" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C14" s="57" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4">
+      <c r="B15" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="C15" s="57" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4">
+      <c r="B16" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C16" s="57" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4">
+      <c r="B17" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C17" s="57" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4">
+      <c r="B18" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="C18" s="57" t="s">
+        <v>157</v>
+      </c>
+      <c r="D18" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4">
+      <c r="B19" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="C19" s="57" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4">
+      <c r="B20" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C20" s="57" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4">
+      <c r="B21" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C21" s="57" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4">
+      <c r="B22" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C22" s="57" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4">
+      <c r="B23" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="C23" s="57" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4">
+      <c r="B24" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C24" s="57" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4">
+      <c r="B25" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C25" s="57"/>
+    </row>
+    <row r="26" spans="2:4">
+      <c r="B26" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C26" s="57" t="s">
+        <v>134</v>
+      </c>
+      <c r="D26" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4">
+      <c r="B27" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="C27" s="57" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4">
+      <c r="B28" s="58" t="s">
+        <v>152</v>
+      </c>
+      <c r="C28" s="57" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4">
+      <c r="B29" s="58" t="s">
+        <v>153</v>
+      </c>
+      <c r="C29" s="57"/>
+    </row>
+    <row r="30" spans="2:4">
+      <c r="B30" s="58" t="s">
+        <v>154</v>
+      </c>
+      <c r="C30" s="57"/>
+    </row>
+    <row r="31" spans="2:4">
+      <c r="B31" s="58" t="s">
+        <v>155</v>
+      </c>
+      <c r="C31" s="57"/>
+    </row>
+    <row r="32" spans="2:4">
+      <c r="B32" s="58" t="s">
+        <v>156</v>
+      </c>
+      <c r="C32" s="57"/>
+    </row>
+    <row r="33" spans="2:4">
+      <c r="B33" s="55" t="s">
+        <v>159</v>
+      </c>
+      <c r="D33" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4">
+      <c r="D35" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4">
+      <c r="D37" t="s">
+        <v>165</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>